<commit_message>
august 13 catch update
</commit_message>
<xml_diff>
--- a/data/fisheries openings 2024.xlsx
+++ b/data/fisheries openings 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="255" documentId="8_{839F1B44-011F-4979-BA54-CC741035DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2177319-FBCE-4BC9-8F25-7FC2AD34F926}"/>
+  <xr:revisionPtr revIDLastSave="260" documentId="8_{839F1B44-011F-4979-BA54-CC741035DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{863DE11D-02F8-4DAB-B789-361A6CD25F77}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="3230" windowWidth="21700" windowHeight="10890" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
+    <workbookView xWindow="11940" yWindow="1680" windowWidth="13280" windowHeight="10890" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeena" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="105">
   <si>
     <t>Gear</t>
   </si>
@@ -286,9 +286,6 @@
     <t>Region 6-Gitksan</t>
   </si>
   <si>
-    <t>Sockeye target</t>
-  </si>
-  <si>
     <t>FN0775</t>
   </si>
   <si>
@@ -347,6 +344,15 @@
   </si>
   <si>
     <t>FN0806</t>
+  </si>
+  <si>
+    <t>FN0809</t>
+  </si>
+  <si>
+    <t>Aug 13-19</t>
+  </si>
+  <si>
+    <t>Sockeye target, selective gear only</t>
   </si>
 </sst>
 </file>
@@ -408,6 +414,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -727,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CF1D5D-9EBE-43D0-AD07-75432409CDE4}">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -841,18 +851,18 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
@@ -867,7 +877,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -878,7 +888,7 @@
         <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -893,7 +903,7 @@
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
@@ -942,7 +952,7 @@
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
@@ -994,7 +1004,7 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
@@ -1020,7 +1030,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -1075,7 +1085,7 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1101,7 +1111,7 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1127,7 +1137,7 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1153,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1251,7 +1261,7 @@
         <v>3</v>
       </c>
       <c r="I20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1277,7 +1287,7 @@
         <v>3</v>
       </c>
       <c r="I21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1303,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1363,13 +1373,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B25" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
         <v>15</v>
@@ -1384,18 +1394,18 @@
         <v>5</v>
       </c>
       <c r="I25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
         <v>60</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
         <v>15</v>
@@ -1410,18 +1420,18 @@
         <v>5</v>
       </c>
       <c r="I26" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B27" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
         <v>15</v>
@@ -1436,7 +1446,7 @@
         <v>5</v>
       </c>
       <c r="I27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
@@ -1462,18 +1472,18 @@
         <v>7</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B29" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D29" t="s">
         <v>15</v>
@@ -1482,21 +1492,21 @@
         <v>36</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B30" t="s">
         <v>37</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" t="s">
         <v>15</v>
@@ -1505,21 +1515,21 @@
         <v>36</v>
       </c>
       <c r="F30" t="s">
+        <v>86</v>
+      </c>
+      <c r="I30" t="s">
         <v>87</v>
-      </c>
-      <c r="I30" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B31" t="s">
         <v>44</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" t="s">
         <v>15</v>
@@ -1534,18 +1544,18 @@
         <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
         <v>60</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D32" t="s">
         <v>15</v>
@@ -1560,18 +1570,18 @@
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
         <v>60</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D33" t="s">
         <v>15</v>
@@ -1586,7 +1596,33 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>96</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>102</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" t="s">
+        <v>61</v>
+      </c>
+      <c r="F34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="I34" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
august 14 update 23
</commit_message>
<xml_diff>
--- a/data/fisheries openings 2024.xlsx
+++ b/data/fisheries openings 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="260" documentId="8_{839F1B44-011F-4979-BA54-CC741035DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{863DE11D-02F8-4DAB-B789-361A6CD25F77}"/>
+  <xr:revisionPtr revIDLastSave="269" documentId="8_{839F1B44-011F-4979-BA54-CC741035DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{135882F8-2807-4DA2-91AA-C33DF23E5A07}"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="1680" windowWidth="13280" windowHeight="10890" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
+    <workbookView xWindow="8590" yWindow="1990" windowWidth="16270" windowHeight="11900" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeena" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
   <si>
     <t>Gear</t>
   </si>
@@ -353,6 +353,15 @@
   </si>
   <si>
     <t>Sockeye target, selective gear only</t>
+  </si>
+  <si>
+    <t>FN0821</t>
+  </si>
+  <si>
+    <t>Aug 15-21</t>
+  </si>
+  <si>
+    <t>Region 6-LBN</t>
   </si>
 </sst>
 </file>
@@ -737,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CF1D5D-9EBE-43D0-AD07-75432409CDE4}">
-  <dimension ref="A1:I34"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C20" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1622,6 +1631,32 @@
         <v>7</v>
       </c>
       <c r="I34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D35" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F35" t="s">
+        <v>107</v>
+      </c>
+      <c r="G35">
+        <v>7</v>
+      </c>
+      <c r="I35" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update fisheries openings table
</commit_message>
<xml_diff>
--- a/data/fisheries openings 2024.xlsx
+++ b/data/fisheries openings 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="269" documentId="8_{839F1B44-011F-4979-BA54-CC741035DE2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{135882F8-2807-4DA2-91AA-C33DF23E5A07}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9356CF0-C251-B446-AF39-32CC3FD4F891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8590" yWindow="1990" windowWidth="16270" windowHeight="11900" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
+    <workbookView xWindow="16080" yWindow="500" windowWidth="24600" windowHeight="16440" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeena" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="111">
   <si>
     <t>Gear</t>
   </si>
@@ -362,6 +362,15 @@
   </si>
   <si>
     <t>Region 6-LBN</t>
+  </si>
+  <si>
+    <t>FN0835</t>
+  </si>
+  <si>
+    <t>Aug 20-26</t>
+  </si>
+  <si>
+    <t>Skeena River - sockeye target, selective gear only</t>
   </si>
 </sst>
 </file>
@@ -423,10 +432,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -746,23 +751,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CF1D5D-9EBE-43D0-AD07-75432409CDE4}">
-  <dimension ref="A1:I35"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
-    <col min="4" max="4" width="11.36328125" customWidth="1"/>
+    <col min="1" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.7265625" customWidth="1"/>
-    <col min="9" max="9" width="22.7265625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -791,7 +796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -814,7 +819,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -837,7 +842,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -863,7 +868,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -889,7 +894,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -915,7 +920,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="80" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -938,7 +943,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -964,7 +969,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -990,7 +995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1016,7 +1021,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1042,7 +1047,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1071,7 +1076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1097,7 +1102,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1123,7 +1128,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1149,7 +1154,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1175,7 +1180,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1198,7 +1203,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1221,7 +1226,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1247,7 +1252,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1273,7 +1278,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1299,7 +1304,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1325,7 +1330,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -1351,7 +1356,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1380,7 +1385,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -1406,7 +1411,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -1432,7 +1437,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1458,7 +1463,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1484,7 +1489,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1507,7 +1512,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1530,7 +1535,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1556,7 +1561,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -1582,7 +1587,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -1608,7 +1613,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -1634,7 +1639,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -1658,6 +1663,32 @@
       </c>
       <c r="I35" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F36" t="s">
+        <v>81</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="I36" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -1676,16 +1707,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.54296875" customWidth="1"/>
-    <col min="3" max="4" width="14.7265625" customWidth="1"/>
-    <col min="6" max="6" width="20.1796875" customWidth="1"/>
-    <col min="7" max="8" width="12.7265625" customWidth="1"/>
-    <col min="9" max="9" width="24.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
+    <col min="3" max="4" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1714,7 +1745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -1740,7 +1771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
andy text update august 27
</commit_message>
<xml_diff>
--- a/data/fisheries openings 2024.xlsx
+++ b/data/fisheries openings 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9356CF0-C251-B446-AF39-32CC3FD4F891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{E9356CF0-C251-B446-AF39-32CC3FD4F891}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1AA679F-09DD-4601-9C30-E7C679A72FD2}"/>
   <bookViews>
-    <workbookView xWindow="16080" yWindow="500" windowWidth="24600" windowHeight="16440" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
+    <workbookView xWindow="1210" yWindow="1840" windowWidth="10970" windowHeight="11900" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeena" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="113">
   <si>
     <t>Gear</t>
   </si>
@@ -361,9 +361,6 @@
     <t>Aug 15-21</t>
   </si>
   <si>
-    <t>Region 6-LBN</t>
-  </si>
-  <si>
     <t>FN0835</t>
   </si>
   <si>
@@ -371,6 +368,15 @@
   </si>
   <si>
     <t>Skeena River - sockeye target, selective gear only</t>
+  </si>
+  <si>
+    <t>FN0853</t>
+  </si>
+  <si>
+    <t>Aug 23-29</t>
+  </si>
+  <si>
+    <t>Region 6-Lake Babine Nation</t>
   </si>
 </sst>
 </file>
@@ -751,23 +757,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CF1D5D-9EBE-43D0-AD07-75432409CDE4}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G15" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="1" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="9" max="9" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -796,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -819,7 +825,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -842,7 +848,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -868,7 +874,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -894,7 +900,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -920,7 +926,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -943,7 +949,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -969,7 +975,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -995,7 +1001,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1021,7 +1027,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1047,7 +1053,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1076,7 +1082,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1102,7 +1108,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1128,7 +1134,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1154,7 +1160,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1180,7 +1186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1203,7 +1209,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1226,7 +1232,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1278,7 +1284,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1304,7 +1310,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1330,7 +1336,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -1356,7 +1362,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1385,7 +1391,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -1411,7 +1417,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -1437,7 +1443,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1463,7 +1469,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1512,7 +1518,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1535,7 +1541,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1561,7 +1567,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -1587,7 +1593,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -1613,7 +1619,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -1639,7 +1645,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -1656,7 +1662,7 @@
         <v>61</v>
       </c>
       <c r="F35" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="G35">
         <v>7</v>
@@ -1665,15 +1671,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="B36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>109</v>
       </c>
       <c r="D36" t="s">
         <v>15</v>
@@ -1688,7 +1694,33 @@
         <v>7</v>
       </c>
       <c r="I36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
         <v>110</v>
+      </c>
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" t="s">
+        <v>61</v>
+      </c>
+      <c r="F37" t="s">
+        <v>112</v>
+      </c>
+      <c r="G37">
+        <v>7</v>
+      </c>
+      <c r="I37" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1707,16 +1739,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="4" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" customWidth="1"/>
+    <col min="9" max="9" width="24.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1745,7 +1777,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -1771,7 +1803,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
andy update sept 15
</commit_message>
<xml_diff>
--- a/data/fisheries openings 2024.xlsx
+++ b/data/fisheries openings 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elh/coastland/skeena-salmon-inseason-updates/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd97481b0ff2b3c9/Documents/R/skeena-sockeye-inseason-updates/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36588398-CA26-0E4D-AF18-5B994E34FC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{36588398-CA26-0E4D-AF18-5B994E34FC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7DE3E83E-17FD-4D4B-92CA-D03941F854B7}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="500" windowWidth="19320" windowHeight="14020" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
+    <workbookView xWindow="6350" yWindow="2760" windowWidth="16270" windowHeight="11900" xr2:uid="{1928A9E5-C03C-4111-994A-5F86A22ABA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Skeena" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="125">
   <si>
     <t>Gear</t>
   </si>
@@ -404,6 +404,15 @@
   </si>
   <si>
     <t>Sept 6-Sept 12</t>
+  </si>
+  <si>
+    <t>Sept 13-19</t>
+  </si>
+  <si>
+    <t>Fulton River ESSR-sockeye target, selective gear only</t>
+  </si>
+  <si>
+    <t>FN0944</t>
   </si>
 </sst>
 </file>
@@ -784,23 +793,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CF1D5D-9EBE-43D0-AD07-75432409CDE4}">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="1" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="14.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.36328125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="9" max="9" width="22.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="9" max="9" width="22.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -829,7 +838,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -852,7 +861,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="64" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -875,7 +884,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -901,7 +910,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -927,7 +936,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -953,7 +962,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="80" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -976,7 +985,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1002,7 +1011,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1028,7 +1037,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1054,7 +1063,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1080,7 +1089,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1109,7 +1118,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -1135,7 +1144,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -1161,7 +1170,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -1187,7 +1196,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>68</v>
       </c>
@@ -1213,7 +1222,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -1259,7 +1268,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -1285,7 +1294,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>71</v>
       </c>
@@ -1311,7 +1320,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>73</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1363,7 +1372,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>75</v>
       </c>
@@ -1389,7 +1398,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>77</v>
       </c>
@@ -1418,7 +1427,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -1444,7 +1453,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>93</v>
       </c>
@@ -1470,7 +1479,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>92</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>79</v>
       </c>
@@ -1522,7 +1531,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -1545,7 +1554,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>85</v>
       </c>
@@ -1568,7 +1577,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>88</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -1620,7 +1629,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>101</v>
       </c>
@@ -1646,7 +1655,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>102</v>
       </c>
@@ -1672,7 +1681,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -1698,7 +1707,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>107</v>
       </c>
@@ -1724,7 +1733,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>110</v>
       </c>
@@ -1750,7 +1759,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>113</v>
       </c>
@@ -1776,7 +1785,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>115</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>117</v>
       </c>
@@ -1828,7 +1837,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>120</v>
       </c>
@@ -1851,7 +1860,33 @@
         <v>7</v>
       </c>
       <c r="I41" t="s">
-        <v>104</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>124</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" t="s">
+        <v>61</v>
+      </c>
+      <c r="F42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42">
+        <v>7</v>
+      </c>
+      <c r="I42" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1870,16 +1905,16 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.5" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" customWidth="1"/>
-    <col min="7" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" customWidth="1"/>
+    <col min="3" max="4" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="20.1796875" customWidth="1"/>
+    <col min="7" max="8" width="12.6328125" customWidth="1"/>
+    <col min="9" max="9" width="24.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1908,7 +1943,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>16</v>
       </c>
@@ -1934,7 +1969,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>

</xml_diff>